<commit_message>
supplemented data from funding tracker
</commit_message>
<xml_diff>
--- a/country_analysis2.xlsx
+++ b/country_analysis2.xlsx
@@ -372,17 +372,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="B3">
@@ -392,37 +392,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Curacao</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B7">
@@ -432,17 +432,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>St. Maarten</t>
+          <t>Curacao</t>
         </is>
       </c>
       <c r="B9">
@@ -452,31 +452,31 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Guyana</t>
         </is>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -492,11 +492,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -512,41 +512,41 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="B16">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="B17">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B18">
-        <v>201</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>St. Maarten</t>
         </is>
       </c>
       <c r="B19">
-        <v>1640</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">

</xml_diff>